<commit_message>
Added operations document Added fornamn and efternamn to internalPerson schema Updated mappings with the new fields Updated mapping documentation
</commit_message>
<xml_diff>
--- a/INT0002.UU.GroupEvents/Src/Files/INT0002.UU.GroupEvents.maps.xlsx
+++ b/INT0002.UU.GroupEvents/Src/Files/INT0002.UU.GroupEvents.maps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AterbudEvent" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="80">
   <si>
     <t>Från</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>/RegistreringEnvelope</t>
+  </si>
+  <si>
+    <t>Fornamn</t>
+  </si>
+  <si>
+    <t>Efternamn</t>
   </si>
 </sst>
 </file>
@@ -352,12 +358,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -366,9 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -381,6 +378,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -682,17 +688,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -715,10 +721,10 @@
       <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -727,8 +733,8 @@
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
@@ -737,8 +743,8 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -747,8 +753,8 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -757,8 +763,8 @@
       <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -767,8 +773,8 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
@@ -789,14 +795,14 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -818,14 +824,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -845,14 +851,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -892,17 +898,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -986,14 +992,14 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1015,14 +1021,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1042,14 +1048,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1086,17 +1092,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1180,14 +1186,14 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1209,14 +1215,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1236,14 +1242,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1276,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,20 +1291,21 @@
     <col min="1" max="1" width="52.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1382,14 +1389,14 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1411,14 +1418,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1438,14 +1445,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1458,9 +1465,22 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
@@ -1479,7 +1499,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D20" sqref="D20:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1491,17 +1511,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1579,14 +1599,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="10" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:4" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1622,32 +1642,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="12" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:4" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14" t="s">
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1676,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1689,17 +1709,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1783,14 +1803,14 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1812,14 +1832,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1839,14 +1859,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1859,12 +1879,22 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C23" s="2"/>
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
@@ -1882,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1895,17 +1925,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -1995,14 +2025,14 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2024,14 +2054,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2051,14 +2081,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2071,12 +2101,22 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C23" s="2"/>
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>

</xml_diff>